<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T07:46:22.252Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24224,9 +24224,69 @@
         <v>8644</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67">
+        <v>77</v>
+      </c>
+      <c r="B67" t="str">
+        <v>16-07-2025 1:16:21 PM</v>
+      </c>
+      <c r="C67" t="str">
+        <v>TN18AA4482</v>
+      </c>
+      <c r="D67" t="str">
+        <v>C099736A</v>
+      </c>
+      <c r="E67" t="str">
+        <v>SKT</v>
+      </c>
+      <c r="F67">
+        <v>11843</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68">
+        <v>78</v>
+      </c>
+      <c r="B68" t="str">
+        <v>16-07-2025 1:16:21 PM</v>
+      </c>
+      <c r="C68" t="str">
+        <v>TN18AA4482</v>
+      </c>
+      <c r="D68" t="str">
+        <v>BCM1421A</v>
+      </c>
+      <c r="E68" t="str">
+        <v>SKT</v>
+      </c>
+      <c r="F68">
+        <v>10652</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69">
+        <v>79</v>
+      </c>
+      <c r="B69" t="str">
+        <v>16-07-2025 1:16:21 PM</v>
+      </c>
+      <c r="C69" t="str">
+        <v>TN18AA4482</v>
+      </c>
+      <c r="D69" t="str">
+        <v>C099796A</v>
+      </c>
+      <c r="E69" t="str">
+        <v>SKT</v>
+      </c>
+      <c r="F69">
+        <v>10244</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F66"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F69"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T07:54:08.937Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24284,9 +24284,69 @@
         <v>10244</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70">
+        <v>80</v>
+      </c>
+      <c r="B70" t="str">
+        <v>16-07-2025 1:24:08 PM</v>
+      </c>
+      <c r="C70" t="str">
+        <v>TN28BD2385</v>
+      </c>
+      <c r="D70" t="str">
+        <v>C099885A</v>
+      </c>
+      <c r="E70" t="str">
+        <v>ASST</v>
+      </c>
+      <c r="F70">
+        <v>11789</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71">
+        <v>81</v>
+      </c>
+      <c r="B71" t="str">
+        <v>16-07-2025 1:24:08 PM</v>
+      </c>
+      <c r="C71" t="str">
+        <v>TN28BD2385</v>
+      </c>
+      <c r="D71" t="str">
+        <v>C063616B</v>
+      </c>
+      <c r="E71" t="str">
+        <v>ASST</v>
+      </c>
+      <c r="F71">
+        <v>10881</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72">
+        <v>82</v>
+      </c>
+      <c r="B72" t="str">
+        <v>16-07-2025 1:24:08 PM</v>
+      </c>
+      <c r="C72" t="str">
+        <v>TN28BD2385</v>
+      </c>
+      <c r="D72" t="str">
+        <v>C065863C</v>
+      </c>
+      <c r="E72" t="str">
+        <v>ASST</v>
+      </c>
+      <c r="F72">
+        <v>8644</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F69"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F72"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T08:02:06.869Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24344,9 +24344,69 @@
         <v>8644</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73">
+        <v>83</v>
+      </c>
+      <c r="B73" t="str">
+        <v>16-07-2025 1:32:06 PM</v>
+      </c>
+      <c r="C73" t="str">
+        <v>TN88L7427</v>
+      </c>
+      <c r="D73" t="str">
+        <v>C065863C</v>
+      </c>
+      <c r="E73" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F73">
+        <v>8644</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74">
+        <v>84</v>
+      </c>
+      <c r="B74" t="str">
+        <v>16-07-2025 1:32:06 PM</v>
+      </c>
+      <c r="C74" t="str">
+        <v>TN88L7427</v>
+      </c>
+      <c r="D74" t="str">
+        <v>C073932A</v>
+      </c>
+      <c r="E74" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F74">
+        <v>8034</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75">
+        <v>85</v>
+      </c>
+      <c r="B75" t="str">
+        <v>16-07-2025 1:32:06 PM</v>
+      </c>
+      <c r="C75" t="str">
+        <v>TN88L7427</v>
+      </c>
+      <c r="D75" t="str">
+        <v>C078741B</v>
+      </c>
+      <c r="E75" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F75">
+        <v>8654</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F72"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F75"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T08:16:13.359Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24404,9 +24404,69 @@
         <v>8654</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76">
+        <v>86</v>
+      </c>
+      <c r="B76" t="str">
+        <v>16-07-2025 1:46:12 PM</v>
+      </c>
+      <c r="C76" t="str">
+        <v>TN04AR8166</v>
+      </c>
+      <c r="D76" t="str">
+        <v>BCL9256A</v>
+      </c>
+      <c r="E76" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F76">
+        <v>10162</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77">
+        <v>87</v>
+      </c>
+      <c r="B77" t="str">
+        <v>16-07-2025 1:46:12 PM</v>
+      </c>
+      <c r="C77" t="str">
+        <v>TN04AR8166</v>
+      </c>
+      <c r="D77" t="str">
+        <v>C061320A</v>
+      </c>
+      <c r="E77" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F77">
+        <v>8599</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78">
+        <v>88</v>
+      </c>
+      <c r="B78" t="str">
+        <v>16-07-2025 1:46:12 PM</v>
+      </c>
+      <c r="C78" t="str">
+        <v>TN04AR8166</v>
+      </c>
+      <c r="D78" t="str">
+        <v>C053304B</v>
+      </c>
+      <c r="E78" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F78">
+        <v>10104</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F75"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F78"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T08:25:38.142Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24464,9 +24464,69 @@
         <v>10104</v>
       </c>
     </row>
+    <row r="79">
+      <c r="A79">
+        <v>89</v>
+      </c>
+      <c r="B79" t="str">
+        <v>16-07-2025 1:55:37 PM</v>
+      </c>
+      <c r="C79" t="str">
+        <v>TN28BD2385</v>
+      </c>
+      <c r="D79" t="str">
+        <v>C093361B</v>
+      </c>
+      <c r="E79" t="str">
+        <v>ASST</v>
+      </c>
+      <c r="F79">
+        <v>9774</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80">
+        <v>90</v>
+      </c>
+      <c r="B80" t="str">
+        <v>16-07-2025 1:55:37 PM</v>
+      </c>
+      <c r="C80" t="str">
+        <v>TN28BD2385</v>
+      </c>
+      <c r="D80" t="str">
+        <v>KGK822A</v>
+      </c>
+      <c r="E80" t="str">
+        <v>ASST</v>
+      </c>
+      <c r="F80">
+        <v>12967</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81">
+        <v>91</v>
+      </c>
+      <c r="B81" t="str">
+        <v>16-07-2025 1:55:37 PM</v>
+      </c>
+      <c r="C81" t="str">
+        <v>TN28BD2385</v>
+      </c>
+      <c r="D81" t="str">
+        <v>BCM1421A</v>
+      </c>
+      <c r="E81" t="str">
+        <v>ASST</v>
+      </c>
+      <c r="F81">
+        <v>10652</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F78"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F81"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T08:53:27.160Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24524,9 +24524,69 @@
         <v>10652</v>
       </c>
     </row>
+    <row r="82">
+      <c r="A82">
+        <v>92</v>
+      </c>
+      <c r="B82" t="str">
+        <v>16-07-2025 2:23:26 PM</v>
+      </c>
+      <c r="C82" t="str">
+        <v>TN04AS5562</v>
+      </c>
+      <c r="D82" t="str">
+        <v>C101527A</v>
+      </c>
+      <c r="E82" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F82">
+        <v>12209</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83">
+        <v>93</v>
+      </c>
+      <c r="B83" t="str">
+        <v>16-07-2025 2:23:26 PM</v>
+      </c>
+      <c r="C83" t="str">
+        <v>TN04AS5562</v>
+      </c>
+      <c r="D83" t="str">
+        <v>C063616C</v>
+      </c>
+      <c r="E83" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F83">
+        <v>11143</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84">
+        <v>94</v>
+      </c>
+      <c r="B84" t="str">
+        <v>16-07-2025 2:23:26 PM</v>
+      </c>
+      <c r="C84" t="str">
+        <v>TN04AS5562</v>
+      </c>
+      <c r="D84" t="str">
+        <v>C064416A</v>
+      </c>
+      <c r="E84" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F84">
+        <v>8511</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F81"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F84"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T09:05:25.767Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24584,9 +24584,69 @@
         <v>8511</v>
       </c>
     </row>
+    <row r="85">
+      <c r="A85">
+        <v>95</v>
+      </c>
+      <c r="B85" t="str">
+        <v>16-07-2025 2:35:25 PM</v>
+      </c>
+      <c r="C85" t="str">
+        <v>TN88H1179</v>
+      </c>
+      <c r="D85" t="str">
+        <v>BCN9423B</v>
+      </c>
+      <c r="E85" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F85">
+        <v>10514</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86">
+        <v>96</v>
+      </c>
+      <c r="B86" t="str">
+        <v>16-07-2025 2:35:25 PM</v>
+      </c>
+      <c r="C86" t="str">
+        <v>TN88H1179</v>
+      </c>
+      <c r="D86" t="str">
+        <v>C065866AA</v>
+      </c>
+      <c r="E86" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F86">
+        <v>7164</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87">
+        <v>97</v>
+      </c>
+      <c r="B87" t="str">
+        <v>16-07-2025 2:35:25 PM</v>
+      </c>
+      <c r="C87" t="str">
+        <v>TN88H1179</v>
+      </c>
+      <c r="D87" t="str">
+        <v>BCK3686</v>
+      </c>
+      <c r="E87" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F87">
+        <v>16851</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F84"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F87"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 2 new entries added on 2025-07-16T09:41:49.854Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24644,9 +24644,49 @@
         <v>16851</v>
       </c>
     </row>
+    <row r="88">
+      <c r="A88">
+        <v>98</v>
+      </c>
+      <c r="B88" t="str">
+        <v>16-07-2025 3:11:49 PM</v>
+      </c>
+      <c r="C88" t="str">
+        <v>TN28BF2542</v>
+      </c>
+      <c r="D88" t="str">
+        <v>BCL6727B</v>
+      </c>
+      <c r="E88" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F88">
+        <v>10802</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89">
+        <v>99</v>
+      </c>
+      <c r="B89" t="str">
+        <v>16-07-2025 3:11:49 PM</v>
+      </c>
+      <c r="C89" t="str">
+        <v>TN28BF2542</v>
+      </c>
+      <c r="D89" t="str">
+        <v>C101168A</v>
+      </c>
+      <c r="E89" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F89">
+        <v>9104</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F87"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F89"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T09:47:23.975Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24684,9 +24684,69 @@
         <v>9104</v>
       </c>
     </row>
+    <row r="90">
+      <c r="A90">
+        <v>100</v>
+      </c>
+      <c r="B90" t="str">
+        <v>16-07-2025 3:17:23 PM</v>
+      </c>
+      <c r="C90" t="str">
+        <v>TN28AK6521</v>
+      </c>
+      <c r="D90" t="str">
+        <v>BCL9256B</v>
+      </c>
+      <c r="E90" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F90">
+        <v>10152</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91">
+        <v>101</v>
+      </c>
+      <c r="B91" t="str">
+        <v>16-07-2025 3:17:23 PM</v>
+      </c>
+      <c r="C91" t="str">
+        <v>TN28AK6521</v>
+      </c>
+      <c r="D91" t="str">
+        <v>BCN7242B</v>
+      </c>
+      <c r="E91" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F91">
+        <v>10181</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92">
+        <v>102</v>
+      </c>
+      <c r="B92" t="str">
+        <v>16-07-2025 3:17:23 PM</v>
+      </c>
+      <c r="C92" t="str">
+        <v>TN28AK6521</v>
+      </c>
+      <c r="D92" t="str">
+        <v>BCM1420A</v>
+      </c>
+      <c r="E92" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F92">
+        <v>14579</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F89"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F92"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T09:59:22.121Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24744,9 +24744,69 @@
         <v>14579</v>
       </c>
     </row>
+    <row r="93">
+      <c r="A93">
+        <v>106</v>
+      </c>
+      <c r="B93" t="str">
+        <v>16-07-2025 3:29:21 PM</v>
+      </c>
+      <c r="C93" t="str">
+        <v>TN04BD5999</v>
+      </c>
+      <c r="D93" t="str">
+        <v>C099736A</v>
+      </c>
+      <c r="E93" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F93">
+        <v>11843</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94">
+        <v>107</v>
+      </c>
+      <c r="B94" t="str">
+        <v>16-07-2025 3:29:21 PM</v>
+      </c>
+      <c r="C94" t="str">
+        <v>TN04BD5999</v>
+      </c>
+      <c r="D94" t="str">
+        <v>C065866AA</v>
+      </c>
+      <c r="E94" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F94">
+        <v>7164</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95">
+        <v>108</v>
+      </c>
+      <c r="B95" t="str">
+        <v>16-07-2025 3:29:21 PM</v>
+      </c>
+      <c r="C95" t="str">
+        <v>TN04BD5999</v>
+      </c>
+      <c r="D95" t="str">
+        <v>C099876A</v>
+      </c>
+      <c r="E95" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F95">
+        <v>12459</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F92"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F95"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T10:04:36.523Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24804,9 +24804,69 @@
         <v>12459</v>
       </c>
     </row>
+    <row r="96">
+      <c r="A96">
+        <v>109</v>
+      </c>
+      <c r="B96" t="str">
+        <v>16-07-2025 3:34:36 PM</v>
+      </c>
+      <c r="C96" t="str">
+        <v>TN18AA4482</v>
+      </c>
+      <c r="D96" t="str">
+        <v>C073932A</v>
+      </c>
+      <c r="E96" t="str">
+        <v>SKT</v>
+      </c>
+      <c r="F96">
+        <v>8034</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97">
+        <v>110</v>
+      </c>
+      <c r="B97" t="str">
+        <v>16-07-2025 3:34:36 PM</v>
+      </c>
+      <c r="C97" t="str">
+        <v>TN18AA4482</v>
+      </c>
+      <c r="D97" t="str">
+        <v>BCL9256B</v>
+      </c>
+      <c r="E97" t="str">
+        <v>SKT</v>
+      </c>
+      <c r="F97">
+        <v>10152</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98">
+        <v>111</v>
+      </c>
+      <c r="B98" t="str">
+        <v>16-07-2025 3:34:36 PM</v>
+      </c>
+      <c r="C98" t="str">
+        <v>TN18AA4482</v>
+      </c>
+      <c r="D98" t="str">
+        <v>BCM1465B</v>
+      </c>
+      <c r="E98" t="str">
+        <v>SKT</v>
+      </c>
+      <c r="F98">
+        <v>14316</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F95"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F98"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T11:00:55.572Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24864,9 +24864,69 @@
         <v>14316</v>
       </c>
     </row>
+    <row r="99">
+      <c r="A99">
+        <v>115</v>
+      </c>
+      <c r="B99" t="str">
+        <v>16-07-2025 4:30:54 PM</v>
+      </c>
+      <c r="C99" t="str">
+        <v>TN04BD9889</v>
+      </c>
+      <c r="D99" t="str">
+        <v>C078812B</v>
+      </c>
+      <c r="E99" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F99">
+        <v>11004</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100">
+        <v>116</v>
+      </c>
+      <c r="B100" t="str">
+        <v>16-07-2025 4:30:54 PM</v>
+      </c>
+      <c r="C100" t="str">
+        <v>TN04BD9889</v>
+      </c>
+      <c r="D100" t="str">
+        <v>C078765B</v>
+      </c>
+      <c r="E100" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F100">
+        <v>11669</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101">
+        <v>117</v>
+      </c>
+      <c r="B101" t="str">
+        <v>16-07-2025 4:30:54 PM</v>
+      </c>
+      <c r="C101" t="str">
+        <v>TN04BD9889</v>
+      </c>
+      <c r="D101" t="str">
+        <v>C099876A</v>
+      </c>
+      <c r="E101" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F101">
+        <v>12459</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F98"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F101"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T11:01:40.183Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -24866,62 +24866,62 @@
     </row>
     <row r="99">
       <c r="A99">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B99" t="str">
-        <v>16-07-2025 4:30:54 PM</v>
+        <v>16-07-2025 4:31:39 PM</v>
       </c>
       <c r="C99" t="str">
-        <v>TN04BD9889</v>
+        <v>TN12AJ8235</v>
       </c>
       <c r="D99" t="str">
-        <v>C078812B</v>
+        <v>BCN6657</v>
       </c>
       <c r="E99" t="str">
-        <v>SJS</v>
+        <v>SVT</v>
       </c>
       <c r="F99">
-        <v>11004</v>
+        <v>13365</v>
       </c>
     </row>
     <row r="100">
       <c r="A100">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B100" t="str">
-        <v>16-07-2025 4:30:54 PM</v>
+        <v>16-07-2025 4:31:39 PM</v>
       </c>
       <c r="C100" t="str">
-        <v>TN04BD9889</v>
+        <v>TN12AJ8235</v>
       </c>
       <c r="D100" t="str">
-        <v>C078765B</v>
+        <v>C078763A</v>
       </c>
       <c r="E100" t="str">
-        <v>SJS</v>
+        <v>SVT</v>
       </c>
       <c r="F100">
-        <v>11669</v>
+        <v>8061</v>
       </c>
     </row>
     <row r="101">
       <c r="A101">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B101" t="str">
-        <v>16-07-2025 4:30:54 PM</v>
+        <v>16-07-2025 4:31:39 PM</v>
       </c>
       <c r="C101" t="str">
-        <v>TN04BD9889</v>
+        <v>TN12AJ8235</v>
       </c>
       <c r="D101" t="str">
-        <v>C099876A</v>
+        <v>C099877A</v>
       </c>
       <c r="E101" t="str">
-        <v>SJS</v>
+        <v>SVT</v>
       </c>
       <c r="F101">
-        <v>12459</v>
+        <v>10145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-17T06:22:25.891Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24924,9 +24924,69 @@
         <v>10145</v>
       </c>
     </row>
+    <row r="102">
+      <c r="A102">
+        <v>118</v>
+      </c>
+      <c r="B102" t="str">
+        <v>17-07-2025 11:52:25 AM</v>
+      </c>
+      <c r="C102" t="str">
+        <v>TN04AJ6985</v>
+      </c>
+      <c r="D102" t="str">
+        <v>C073931A</v>
+      </c>
+      <c r="E102" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F102">
+        <v>8564</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103">
+        <v>119</v>
+      </c>
+      <c r="B103" t="str">
+        <v>17-07-2025 11:52:25 AM</v>
+      </c>
+      <c r="C103" t="str">
+        <v>TN04AJ6985</v>
+      </c>
+      <c r="D103" t="str">
+        <v>BCM1421B</v>
+      </c>
+      <c r="E103" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F103">
+        <v>10652</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104">
+        <v>120</v>
+      </c>
+      <c r="B104" t="str">
+        <v>17-07-2025 11:52:25 AM</v>
+      </c>
+      <c r="C104" t="str">
+        <v>TN04AJ6985</v>
+      </c>
+      <c r="D104" t="str">
+        <v>BCN2078A</v>
+      </c>
+      <c r="E104" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F104">
+        <v>7635</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F101"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F104"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-17T06:35:59.658Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F107"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24984,9 +24984,69 @@
         <v>7635</v>
       </c>
     </row>
+    <row r="105">
+      <c r="A105">
+        <v>121</v>
+      </c>
+      <c r="B105" t="str">
+        <v>17-07-2025 12:05:59 PM</v>
+      </c>
+      <c r="C105" t="str">
+        <v>TN04AY7520</v>
+      </c>
+      <c r="D105" t="str">
+        <v>C100525B</v>
+      </c>
+      <c r="E105" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F105">
+        <v>9988</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106">
+        <v>122</v>
+      </c>
+      <c r="B106" t="str">
+        <v>17-07-2025 12:05:59 PM</v>
+      </c>
+      <c r="C106" t="str">
+        <v>TN04AY7520</v>
+      </c>
+      <c r="D106" t="str">
+        <v>C096391A</v>
+      </c>
+      <c r="E106" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F106">
+        <v>10951</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107">
+        <v>123</v>
+      </c>
+      <c r="B107" t="str">
+        <v>17-07-2025 12:05:59 PM</v>
+      </c>
+      <c r="C107" t="str">
+        <v>TN04AY7520</v>
+      </c>
+      <c r="D107" t="str">
+        <v>C078741B</v>
+      </c>
+      <c r="E107" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F107">
+        <v>8654</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F104"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F107"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-17T06:44:57.985Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F107"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25044,9 +25044,69 @@
         <v>8654</v>
       </c>
     </row>
+    <row r="108">
+      <c r="A108">
+        <v>124</v>
+      </c>
+      <c r="B108" t="str">
+        <v>17-07-2025 12:14:57 PM</v>
+      </c>
+      <c r="C108" t="str">
+        <v>TN04AY8968</v>
+      </c>
+      <c r="D108" t="str">
+        <v>BCL9256B</v>
+      </c>
+      <c r="E108" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F108">
+        <v>10152</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109">
+        <v>125</v>
+      </c>
+      <c r="B109" t="str">
+        <v>17-07-2025 12:14:57 PM</v>
+      </c>
+      <c r="C109" t="str">
+        <v>TN04AY8968</v>
+      </c>
+      <c r="D109" t="str">
+        <v>C063616B</v>
+      </c>
+      <c r="E109" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F109">
+        <v>10881</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110">
+        <v>126</v>
+      </c>
+      <c r="B110" t="str">
+        <v>17-07-2025 12:14:57 PM</v>
+      </c>
+      <c r="C110" t="str">
+        <v>TN04AY8968</v>
+      </c>
+      <c r="D110" t="str">
+        <v>C064415C</v>
+      </c>
+      <c r="E110" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F110">
+        <v>8271</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F107"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F110"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-17T08:29:39.861Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:F113"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25104,9 +25104,69 @@
         <v>8271</v>
       </c>
     </row>
+    <row r="111">
+      <c r="A111">
+        <v>127</v>
+      </c>
+      <c r="B111" t="str">
+        <v>17-07-2025 1:59:39 PM</v>
+      </c>
+      <c r="C111" t="str">
+        <v>TN04AR3918</v>
+      </c>
+      <c r="D111" t="str">
+        <v>AS35147B</v>
+      </c>
+      <c r="E111" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F111">
+        <v>11333</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112">
+        <v>128</v>
+      </c>
+      <c r="B112" t="str">
+        <v>17-07-2025 1:59:39 PM</v>
+      </c>
+      <c r="C112" t="str">
+        <v>TN04AR3918</v>
+      </c>
+      <c r="D112" t="str">
+        <v>C098572A</v>
+      </c>
+      <c r="E112" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F112">
+        <v>11851</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113">
+        <v>129</v>
+      </c>
+      <c r="B113" t="str">
+        <v>17-07-2025 1:59:39 PM</v>
+      </c>
+      <c r="C113" t="str">
+        <v>TN04AR3918</v>
+      </c>
+      <c r="D113" t="str">
+        <v>C093361B</v>
+      </c>
+      <c r="E113" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F113">
+        <v>9774</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F110"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F113"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-17T09:40:31.570Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F113"/>
+  <dimension ref="A1:F116"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25164,9 +25164,69 @@
         <v>9774</v>
       </c>
     </row>
+    <row r="114">
+      <c r="A114">
+        <v>133</v>
+      </c>
+      <c r="B114" t="str">
+        <v>17-07-2025 3:10:30 PM</v>
+      </c>
+      <c r="C114" t="str">
+        <v>TN04AR8166</v>
+      </c>
+      <c r="D114" t="str">
+        <v>BCN6657</v>
+      </c>
+      <c r="E114" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F114">
+        <v>13365</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115">
+        <v>134</v>
+      </c>
+      <c r="B115" t="str">
+        <v>17-07-2025 3:10:30 PM</v>
+      </c>
+      <c r="C115" t="str">
+        <v>TN04AR8166</v>
+      </c>
+      <c r="D115" t="str">
+        <v>C065863B</v>
+      </c>
+      <c r="E115" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F115">
+        <v>8614</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116">
+        <v>135</v>
+      </c>
+      <c r="B116" t="str">
+        <v>17-07-2025 3:10:30 PM</v>
+      </c>
+      <c r="C116" t="str">
+        <v>TN04AR8166</v>
+      </c>
+      <c r="D116" t="str">
+        <v>C057810A</v>
+      </c>
+      <c r="E116" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F116">
+        <v>11841</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F113"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F116"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 4 new entries added on 2025-07-17T09:41:40.154Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F116"/>
+  <dimension ref="A1:F117"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25166,67 +25166,87 @@
     </row>
     <row r="114">
       <c r="A114">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B114" t="str">
-        <v>17-07-2025 3:10:30 PM</v>
+        <v>17-07-2025 3:11:39 PM</v>
       </c>
       <c r="C114" t="str">
-        <v>TN04AR8166</v>
+        <v>TN03AK4570</v>
       </c>
       <c r="D114" t="str">
-        <v>BCN6657</v>
+        <v>BCJ6408B</v>
       </c>
       <c r="E114" t="str">
-        <v>GWS</v>
+        <v>MST</v>
       </c>
       <c r="F114">
-        <v>13365</v>
+        <v>12040</v>
       </c>
     </row>
     <row r="115">
       <c r="A115">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B115" t="str">
-        <v>17-07-2025 3:10:30 PM</v>
+        <v>17-07-2025 3:11:39 PM</v>
       </c>
       <c r="C115" t="str">
-        <v>TN04AR8166</v>
+        <v>TN03AK4570</v>
       </c>
       <c r="D115" t="str">
-        <v>C065863B</v>
+        <v>C068459</v>
       </c>
       <c r="E115" t="str">
-        <v>GWS</v>
+        <v>MST</v>
       </c>
       <c r="F115">
-        <v>8614</v>
+        <v>6980</v>
       </c>
     </row>
     <row r="116">
       <c r="A116">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B116" t="str">
-        <v>17-07-2025 3:10:30 PM</v>
+        <v>17-07-2025 3:11:39 PM</v>
       </c>
       <c r="C116" t="str">
-        <v>TN04AR8166</v>
+        <v>TN03AK4570</v>
       </c>
       <c r="D116" t="str">
-        <v>C057810A</v>
+        <v>C087506B</v>
       </c>
       <c r="E116" t="str">
-        <v>GWS</v>
+        <v>MST</v>
       </c>
       <c r="F116">
-        <v>11841</v>
+        <v>11159</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117">
+        <v>133</v>
+      </c>
+      <c r="B117" t="str">
+        <v>17-07-2025 3:11:39 PM</v>
+      </c>
+      <c r="C117" t="str">
+        <v>TN03AK4570</v>
+      </c>
+      <c r="D117" t="str">
+        <v>C065864A</v>
+      </c>
+      <c r="E117" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F117">
+        <v>8764</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F116"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F117"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-17T10:02:13.834Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F117"/>
+  <dimension ref="A1:F120"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25244,9 +25244,69 @@
         <v>8764</v>
       </c>
     </row>
+    <row r="118">
+      <c r="A118">
+        <v>137</v>
+      </c>
+      <c r="B118" t="str">
+        <v>17-07-2025 3:32:13 PM</v>
+      </c>
+      <c r="C118" t="str">
+        <v>TN18R1273</v>
+      </c>
+      <c r="D118" t="str">
+        <v>BCN2078B</v>
+      </c>
+      <c r="E118" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F118">
+        <v>7635</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119">
+        <v>138</v>
+      </c>
+      <c r="B119" t="str">
+        <v>17-07-2025 3:32:13 PM</v>
+      </c>
+      <c r="C119" t="str">
+        <v>TN18R1273</v>
+      </c>
+      <c r="D119" t="str">
+        <v>C087504B</v>
+      </c>
+      <c r="E119" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F119">
+        <v>9615</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120">
+        <v>139</v>
+      </c>
+      <c r="B120" t="str">
+        <v>17-07-2025 3:32:13 PM</v>
+      </c>
+      <c r="C120" t="str">
+        <v>TN18R1273</v>
+      </c>
+      <c r="D120" t="str">
+        <v>C099798B</v>
+      </c>
+      <c r="E120" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F120">
+        <v>10054</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F117"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F120"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-17T10:28:59.297Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F120"/>
+  <dimension ref="A1:F123"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25304,9 +25304,69 @@
         <v>10054</v>
       </c>
     </row>
+    <row r="121">
+      <c r="A121">
+        <v>140</v>
+      </c>
+      <c r="B121" t="str">
+        <v>17-07-2025 3:58:58 PM</v>
+      </c>
+      <c r="C121" t="str">
+        <v>TN03J6473</v>
+      </c>
+      <c r="D121" t="str">
+        <v>BCL9256A</v>
+      </c>
+      <c r="E121" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F121">
+        <v>10162</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122">
+        <v>141</v>
+      </c>
+      <c r="B122" t="str">
+        <v>17-07-2025 3:58:58 PM</v>
+      </c>
+      <c r="C122" t="str">
+        <v>TN03J6473</v>
+      </c>
+      <c r="D122" t="str">
+        <v>C065863A</v>
+      </c>
+      <c r="E122" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F122">
+        <v>8614</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123">
+        <v>142</v>
+      </c>
+      <c r="B123" t="str">
+        <v>17-07-2025 3:58:58 PM</v>
+      </c>
+      <c r="C123" t="str">
+        <v>TN03J6473</v>
+      </c>
+      <c r="D123" t="str">
+        <v>C101233B</v>
+      </c>
+      <c r="E123" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F123">
+        <v>11159</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F120"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F123"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-17T10:39:40.439Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F123"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25364,9 +25364,69 @@
         <v>11159</v>
       </c>
     </row>
+    <row r="124">
+      <c r="A124">
+        <v>143</v>
+      </c>
+      <c r="B124" t="str">
+        <v>17-07-2025 4:09:40 PM</v>
+      </c>
+      <c r="C124" t="str">
+        <v>TN04AJ9783</v>
+      </c>
+      <c r="D124" t="str">
+        <v>BCL9256B</v>
+      </c>
+      <c r="E124" t="str">
+        <v>MSMD</v>
+      </c>
+      <c r="F124">
+        <v>10152</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125">
+        <v>144</v>
+      </c>
+      <c r="B125" t="str">
+        <v>17-07-2025 4:09:40 PM</v>
+      </c>
+      <c r="C125" t="str">
+        <v>TN04AJ9783</v>
+      </c>
+      <c r="D125" t="str">
+        <v>BCN9423A</v>
+      </c>
+      <c r="E125" t="str">
+        <v>MSMD</v>
+      </c>
+      <c r="F125">
+        <v>10934</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126">
+        <v>145</v>
+      </c>
+      <c r="B126" t="str">
+        <v>17-07-2025 4:09:40 PM</v>
+      </c>
+      <c r="C126" t="str">
+        <v>TN04AJ9783</v>
+      </c>
+      <c r="D126" t="str">
+        <v>C062523A</v>
+      </c>
+      <c r="E126" t="str">
+        <v>MSMD</v>
+      </c>
+      <c r="F126">
+        <v>10574</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F123"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F126"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-17T10:40:54.659Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -25366,62 +25366,62 @@
     </row>
     <row r="124">
       <c r="A124">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B124" t="str">
-        <v>17-07-2025 4:09:40 PM</v>
+        <v>17-07-2025 4:10:53 PM</v>
       </c>
       <c r="C124" t="str">
-        <v>TN04AJ9783</v>
+        <v>TN04AR8166</v>
       </c>
       <c r="D124" t="str">
-        <v>BCL9256B</v>
+        <v>BCL9258A</v>
       </c>
       <c r="E124" t="str">
-        <v>MSMD</v>
+        <v>GWS</v>
       </c>
       <c r="F124">
-        <v>10152</v>
+        <v>10502</v>
       </c>
     </row>
     <row r="125">
       <c r="A125">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B125" t="str">
-        <v>17-07-2025 4:09:40 PM</v>
+        <v>17-07-2025 4:10:53 PM</v>
       </c>
       <c r="C125" t="str">
-        <v>TN04AJ9783</v>
+        <v>TN04AR8166</v>
       </c>
       <c r="D125" t="str">
-        <v>BCN9423A</v>
+        <v>KGK695A</v>
       </c>
       <c r="E125" t="str">
-        <v>MSMD</v>
+        <v>GWS</v>
       </c>
       <c r="F125">
-        <v>10934</v>
+        <v>12443</v>
       </c>
     </row>
     <row r="126">
       <c r="A126">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B126" t="str">
-        <v>17-07-2025 4:09:40 PM</v>
+        <v>17-07-2025 4:10:53 PM</v>
       </c>
       <c r="C126" t="str">
-        <v>TN04AJ9783</v>
+        <v>TN04AR8166</v>
       </c>
       <c r="D126" t="str">
-        <v>C062523A</v>
+        <v>C080047A</v>
       </c>
       <c r="E126" t="str">
-        <v>MSMD</v>
+        <v>GWS</v>
       </c>
       <c r="F126">
-        <v>10574</v>
+        <v>8627</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-17T10:57:57.408Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25424,9 +25424,69 @@
         <v>8627</v>
       </c>
     </row>
+    <row r="127">
+      <c r="A127">
+        <v>149</v>
+      </c>
+      <c r="B127" t="str">
+        <v>17-07-2025 4:27:57 PM</v>
+      </c>
+      <c r="C127" t="str">
+        <v>TN04AJ6982</v>
+      </c>
+      <c r="D127" t="str">
+        <v>BCL9256A</v>
+      </c>
+      <c r="E127" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F127">
+        <v>10162</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128">
+        <v>150</v>
+      </c>
+      <c r="B128" t="str">
+        <v>17-07-2025 4:27:57 PM</v>
+      </c>
+      <c r="C128" t="str">
+        <v>TN04AJ6982</v>
+      </c>
+      <c r="D128" t="str">
+        <v>C065863C</v>
+      </c>
+      <c r="E128" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F128">
+        <v>8644</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129">
+        <v>151</v>
+      </c>
+      <c r="B129" t="str">
+        <v>17-07-2025 4:27:57 PM</v>
+      </c>
+      <c r="C129" t="str">
+        <v>TN04AJ6982</v>
+      </c>
+      <c r="D129" t="str">
+        <v>BCM6891B</v>
+      </c>
+      <c r="E129" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F129">
+        <v>8865</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F126"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F129"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 5 new entries added on 2025-07-17T11:16:06.141Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25484,9 +25484,109 @@
         <v>8865</v>
       </c>
     </row>
+    <row r="130">
+      <c r="A130">
+        <v>152</v>
+      </c>
+      <c r="B130" t="str">
+        <v>17-07-2025 4:46:04 PM</v>
+      </c>
+      <c r="C130" t="str">
+        <v>TN04AB5676</v>
+      </c>
+      <c r="D130" t="str">
+        <v>C078763A</v>
+      </c>
+      <c r="E130" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F130">
+        <v>8061</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131">
+        <v>153</v>
+      </c>
+      <c r="B131" t="str">
+        <v>17-07-2025 4:46:04 PM</v>
+      </c>
+      <c r="C131" t="str">
+        <v>TN04AB5676</v>
+      </c>
+      <c r="D131" t="str">
+        <v>BCN2078B</v>
+      </c>
+      <c r="E131" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F131">
+        <v>7635</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132">
+        <v>154</v>
+      </c>
+      <c r="B132" t="str">
+        <v>17-07-2025 4:46:04 PM</v>
+      </c>
+      <c r="C132" t="str">
+        <v>TN04AB5676</v>
+      </c>
+      <c r="D132" t="str">
+        <v>BCM6773C</v>
+      </c>
+      <c r="E132" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F132">
+        <v>7321</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133">
+        <v>155</v>
+      </c>
+      <c r="B133" t="str">
+        <v>17-07-2025 4:46:04 PM</v>
+      </c>
+      <c r="C133" t="str">
+        <v>TN04AB5676</v>
+      </c>
+      <c r="D133" t="str">
+        <v>C068459</v>
+      </c>
+      <c r="E133" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F133">
+        <v>6980</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134">
+        <v>156</v>
+      </c>
+      <c r="B134" t="str">
+        <v>17-07-2025 4:46:04 PM</v>
+      </c>
+      <c r="C134" t="str">
+        <v>TN04AB5676</v>
+      </c>
+      <c r="D134" t="str">
+        <v>C065863B</v>
+      </c>
+      <c r="E134" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F134">
+        <v>8614</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F129"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F134"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-17T11:25:31.176Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25584,9 +25584,69 @@
         <v>8614</v>
       </c>
     </row>
+    <row r="135">
+      <c r="A135">
+        <v>157</v>
+      </c>
+      <c r="B135" t="str">
+        <v>17-07-2025 4:55:30 PM</v>
+      </c>
+      <c r="C135" t="str">
+        <v>TN04AB5676</v>
+      </c>
+      <c r="D135" t="str">
+        <v>C078763A</v>
+      </c>
+      <c r="E135" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F135">
+        <v>8061</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136">
+        <v>158</v>
+      </c>
+      <c r="B136" t="str">
+        <v>17-07-2025 4:55:30 PM</v>
+      </c>
+      <c r="C136" t="str">
+        <v>TN04AB5676</v>
+      </c>
+      <c r="D136" t="str">
+        <v>BCL7865</v>
+      </c>
+      <c r="E136" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F136">
+        <v>18165</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137">
+        <v>159</v>
+      </c>
+      <c r="B137" t="str">
+        <v>17-07-2025 4:55:30 PM</v>
+      </c>
+      <c r="C137" t="str">
+        <v>TN04AB5676</v>
+      </c>
+      <c r="D137" t="str">
+        <v>BCM6773C</v>
+      </c>
+      <c r="E137" t="str">
+        <v>SJS</v>
+      </c>
+      <c r="F137">
+        <v>7321</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F134"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F137"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 4 new entries added on 2025-07-18T05:13:27.649Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F137"/>
+  <dimension ref="A1:F141"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25644,9 +25644,89 @@
         <v>7321</v>
       </c>
     </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>160.1</v>
+      </c>
+      <c r="B138" t="str">
+        <v>18-07-2025 10:43:27 AM</v>
+      </c>
+      <c r="C138" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D138" t="str">
+        <v>BCL9256A</v>
+      </c>
+      <c r="E138" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F138">
+        <v>10162</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>160.2</v>
+      </c>
+      <c r="B139" t="str">
+        <v>18-07-2025 10:43:27 AM</v>
+      </c>
+      <c r="C139" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D139" t="str">
+        <v>C099796A</v>
+      </c>
+      <c r="E139" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F139">
+        <v>10244</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>160.3</v>
+      </c>
+      <c r="B140" t="str">
+        <v>18-07-2025 10:43:27 AM</v>
+      </c>
+      <c r="C140" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D140" t="str">
+        <v>BCM4941B</v>
+      </c>
+      <c r="E140" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F140">
+        <v>8561</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>160.4</v>
+      </c>
+      <c r="B141" t="str">
+        <v>18-07-2025 10:43:27 AM</v>
+      </c>
+      <c r="C141" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D141" t="str">
+        <v>BCM8546B</v>
+      </c>
+      <c r="E141" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F141">
+        <v>8435</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F137"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F141"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T05:37:22.751Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F141"/>
+  <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25724,9 +25724,69 @@
         <v>8435</v>
       </c>
     </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>161.1</v>
+      </c>
+      <c r="B142" t="str">
+        <v>18-07-2025 11:07:21 AM</v>
+      </c>
+      <c r="C142" t="str">
+        <v>TN28AK6521</v>
+      </c>
+      <c r="D142" t="str">
+        <v>BCM6772B</v>
+      </c>
+      <c r="E142" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F142">
+        <v>9965</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>161.2</v>
+      </c>
+      <c r="B143" t="str">
+        <v>18-07-2025 11:07:21 AM</v>
+      </c>
+      <c r="C143" t="str">
+        <v>TN28AK6521</v>
+      </c>
+      <c r="D143" t="str">
+        <v>C068459</v>
+      </c>
+      <c r="E143" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F143">
+        <v>6980</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v>161.3</v>
+      </c>
+      <c r="B144" t="str">
+        <v>18-07-2025 11:07:21 AM</v>
+      </c>
+      <c r="C144" t="str">
+        <v>TN28AK6521</v>
+      </c>
+      <c r="D144" t="str">
+        <v>C101291B</v>
+      </c>
+      <c r="E144" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F144">
+        <v>9281</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F141"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F144"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T05:46:44.760Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F144"/>
+  <dimension ref="A1:F147"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25784,9 +25784,69 @@
         <v>9281</v>
       </c>
     </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v>1.1</v>
+      </c>
+      <c r="B145" t="str">
+        <v>18-07-2025 11:16:44 AM</v>
+      </c>
+      <c r="C145" t="str">
+        <v>TN88L5807</v>
+      </c>
+      <c r="D145" t="str">
+        <v>BCL9256B</v>
+      </c>
+      <c r="E145" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F145">
+        <v>10152</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v>1.2</v>
+      </c>
+      <c r="B146" t="str">
+        <v>18-07-2025 11:16:44 AM</v>
+      </c>
+      <c r="C146" t="str">
+        <v>TN88L5807</v>
+      </c>
+      <c r="D146" t="str">
+        <v>C057819B</v>
+      </c>
+      <c r="E146" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F146">
+        <v>8164</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>1.3</v>
+      </c>
+      <c r="B147" t="str">
+        <v>18-07-2025 11:16:44 AM</v>
+      </c>
+      <c r="C147" t="str">
+        <v>TN88L5807</v>
+      </c>
+      <c r="D147" t="str">
+        <v>C064415C</v>
+      </c>
+      <c r="E147" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F147">
+        <v>8271</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F144"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F147"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T05:49:18.090Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -25786,19 +25786,19 @@
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>1.1</v>
+        <v>2.1</v>
       </c>
       <c r="B145" t="str">
-        <v>18-07-2025 11:16:44 AM</v>
+        <v>18-07-2025 11:19:17 AM</v>
       </c>
       <c r="C145" t="str">
-        <v>TN88L5807</v>
+        <v>TN28BA6503</v>
       </c>
       <c r="D145" t="str">
         <v>BCL9256B</v>
       </c>
       <c r="E145" t="str">
-        <v>MPT</v>
+        <v>JPM</v>
       </c>
       <c r="F145">
         <v>10152</v>
@@ -25806,42 +25806,42 @@
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>1.2</v>
+        <v>2.2</v>
       </c>
       <c r="B146" t="str">
-        <v>18-07-2025 11:16:44 AM</v>
+        <v>18-07-2025 11:19:17 AM</v>
       </c>
       <c r="C146" t="str">
-        <v>TN88L5807</v>
+        <v>TN28BA6503</v>
       </c>
       <c r="D146" t="str">
-        <v>C057819B</v>
+        <v>BCN7242A</v>
       </c>
       <c r="E146" t="str">
-        <v>MPT</v>
+        <v>JPM</v>
       </c>
       <c r="F146">
-        <v>8164</v>
+        <v>10171</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>1.3</v>
+        <v>2.3</v>
       </c>
       <c r="B147" t="str">
-        <v>18-07-2025 11:16:44 AM</v>
+        <v>18-07-2025 11:19:17 AM</v>
       </c>
       <c r="C147" t="str">
-        <v>TN88L5807</v>
+        <v>TN28BA6503</v>
       </c>
       <c r="D147" t="str">
-        <v>C064415C</v>
+        <v>C101168A</v>
       </c>
       <c r="E147" t="str">
-        <v>MPT</v>
+        <v>JPM</v>
       </c>
       <c r="F147">
-        <v>8271</v>
+        <v>9104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T05:57:09.194Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F147"/>
+  <dimension ref="A1:F150"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25844,9 +25844,69 @@
         <v>9104</v>
       </c>
     </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v>3.1</v>
+      </c>
+      <c r="B148" t="str">
+        <v>18-07-2025 11:26:11 AM</v>
+      </c>
+      <c r="C148" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D148" t="str">
+        <v>C100714A</v>
+      </c>
+      <c r="E148" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F148">
+        <v>9294</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <v>3.2</v>
+      </c>
+      <c r="B149" t="str">
+        <v>18-07-2025 11:26:11 AM</v>
+      </c>
+      <c r="C149" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D149" t="str">
+        <v>C093361B</v>
+      </c>
+      <c r="E149" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F149">
+        <v>9774</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <v>3.3</v>
+      </c>
+      <c r="B150" t="str">
+        <v>18-07-2025 11:26:11 AM</v>
+      </c>
+      <c r="C150" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D150" t="str">
+        <v>C078763B</v>
+      </c>
+      <c r="E150" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F150">
+        <v>8061</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F147"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F150"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T06:10:24.120Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F150"/>
+  <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25904,9 +25904,69 @@
         <v>8061</v>
       </c>
     </row>
+    <row r="151">
+      <c r="A151" t="str">
+        <v>1.1</v>
+      </c>
+      <c r="B151" t="str">
+        <v>18-07-2025 11:40:23 AM</v>
+      </c>
+      <c r="C151" t="str">
+        <v>TN28AK9553</v>
+      </c>
+      <c r="D151" t="str">
+        <v>BCL9258B</v>
+      </c>
+      <c r="E151" t="str">
+        <v>SCT</v>
+      </c>
+      <c r="F151">
+        <v>10492</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="str">
+        <v>1.2</v>
+      </c>
+      <c r="B152" t="str">
+        <v>18-07-2025 11:40:23 AM</v>
+      </c>
+      <c r="C152" t="str">
+        <v>TN28AK9553</v>
+      </c>
+      <c r="D152" t="str">
+        <v>BCL9256B</v>
+      </c>
+      <c r="E152" t="str">
+        <v>SCT</v>
+      </c>
+      <c r="F152">
+        <v>10152</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="str">
+        <v>1.3</v>
+      </c>
+      <c r="B153" t="str">
+        <v>18-07-2025 11:40:23 AM</v>
+      </c>
+      <c r="C153" t="str">
+        <v>TN28AK9553</v>
+      </c>
+      <c r="D153" t="str">
+        <v>BCM8546C</v>
+      </c>
+      <c r="E153" t="str">
+        <v>SCT</v>
+      </c>
+      <c r="F153">
+        <v>8235</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F150"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F153"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T06:22:12.555Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F153"/>
+  <dimension ref="A1:F156"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -25964,9 +25964,69 @@
         <v>8235</v>
       </c>
     </row>
+    <row r="154">
+      <c r="A154" t="str">
+        <v>1.1</v>
+      </c>
+      <c r="B154" t="str">
+        <v>18-07-2025 11:52:11 AM</v>
+      </c>
+      <c r="C154" t="str">
+        <v>TN04AS5548</v>
+      </c>
+      <c r="D154" t="str">
+        <v>BCM6772B</v>
+      </c>
+      <c r="E154" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F154">
+        <v>9965</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="str">
+        <v>1.2</v>
+      </c>
+      <c r="B155" t="str">
+        <v>18-07-2025 11:52:11 AM</v>
+      </c>
+      <c r="C155" t="str">
+        <v>TN04AS5548</v>
+      </c>
+      <c r="D155" t="str">
+        <v>C064416A</v>
+      </c>
+      <c r="E155" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F155">
+        <v>8511</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="str">
+        <v>1.3</v>
+      </c>
+      <c r="B156" t="str">
+        <v>18-07-2025 11:52:11 AM</v>
+      </c>
+      <c r="C156" t="str">
+        <v>TN04AS5548</v>
+      </c>
+      <c r="D156" t="str">
+        <v>C063616A</v>
+      </c>
+      <c r="E156" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F156">
+        <v>10881</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F153"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F156"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T06:29:20.486Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F156"/>
+  <dimension ref="A1:F159"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -26024,9 +26024,69 @@
         <v>10881</v>
       </c>
     </row>
+    <row r="157">
+      <c r="A157" t="str">
+        <v>1.1</v>
+      </c>
+      <c r="B157" t="str">
+        <v>18-07-2025 11:59:19 AM</v>
+      </c>
+      <c r="C157" t="str">
+        <v>TN28BA6503</v>
+      </c>
+      <c r="D157" t="str">
+        <v>BCM0846A</v>
+      </c>
+      <c r="E157" t="str">
+        <v>JPM</v>
+      </c>
+      <c r="F157">
+        <v>10614</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="str">
+        <v>1.2</v>
+      </c>
+      <c r="B158" t="str">
+        <v>18-07-2025 11:59:19 AM</v>
+      </c>
+      <c r="C158" t="str">
+        <v>TN28BA6503</v>
+      </c>
+      <c r="D158" t="str">
+        <v>C082138A</v>
+      </c>
+      <c r="E158" t="str">
+        <v>JPM</v>
+      </c>
+      <c r="F158">
+        <v>10694</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="str">
+        <v>1.3</v>
+      </c>
+      <c r="B159" t="str">
+        <v>18-07-2025 11:59:19 AM</v>
+      </c>
+      <c r="C159" t="str">
+        <v>TN28BA6503</v>
+      </c>
+      <c r="D159" t="str">
+        <v>C073931A</v>
+      </c>
+      <c r="E159" t="str">
+        <v>JPM</v>
+      </c>
+      <c r="F159">
+        <v>8564</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F156"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F159"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T06:46:46.182Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F159"/>
+  <dimension ref="A1:F162"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -26084,9 +26084,69 @@
         <v>8564</v>
       </c>
     </row>
+    <row r="160">
+      <c r="A160" t="str">
+        <v>1.1</v>
+      </c>
+      <c r="B160" t="str">
+        <v>18-07-2025 12:16:44 PM</v>
+      </c>
+      <c r="C160" t="str">
+        <v>TN28BD1127</v>
+      </c>
+      <c r="D160" t="str">
+        <v>BCN9154C</v>
+      </c>
+      <c r="E160" t="str">
+        <v>JPM</v>
+      </c>
+      <c r="F160">
+        <v>10952</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="str">
+        <v>1.2</v>
+      </c>
+      <c r="B161" t="str">
+        <v>18-07-2025 12:16:44 PM</v>
+      </c>
+      <c r="C161" t="str">
+        <v>TN28BD1127</v>
+      </c>
+      <c r="D161" t="str">
+        <v>BCL9258C</v>
+      </c>
+      <c r="E161" t="str">
+        <v>JPM</v>
+      </c>
+      <c r="F161">
+        <v>10842</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="str">
+        <v>1.3</v>
+      </c>
+      <c r="B162" t="str">
+        <v>18-07-2025 12:16:44 PM</v>
+      </c>
+      <c r="C162" t="str">
+        <v>TN28BD1127</v>
+      </c>
+      <c r="D162" t="str">
+        <v>BCM8546A</v>
+      </c>
+      <c r="E162" t="str">
+        <v>JPM</v>
+      </c>
+      <c r="F162">
+        <v>8445</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F159"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F162"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T07:49:19.727Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F162"/>
+  <dimension ref="A1:F165"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -26144,9 +26144,69 @@
         <v>8445</v>
       </c>
     </row>
+    <row r="163">
+      <c r="A163" t="str">
+        <v>1.1</v>
+      </c>
+      <c r="B163" t="str">
+        <v>18-07-2025 1:19:19 PM</v>
+      </c>
+      <c r="C163" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D163" t="str">
+        <v>C099793A</v>
+      </c>
+      <c r="E163" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F163">
+        <v>10244</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="str">
+        <v>1.2</v>
+      </c>
+      <c r="B164" t="str">
+        <v>18-07-2025 1:19:19 PM</v>
+      </c>
+      <c r="C164" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D164" t="str">
+        <v>C065037A</v>
+      </c>
+      <c r="E164" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F164">
+        <v>9714</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="str">
+        <v>1.3</v>
+      </c>
+      <c r="B165" t="str">
+        <v>18-07-2025 1:19:19 PM</v>
+      </c>
+      <c r="C165" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D165" t="str">
+        <v>BCM4459B</v>
+      </c>
+      <c r="E165" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F165">
+        <v>8805</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F162"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F165"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T07:58:45.211Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F165"/>
+  <dimension ref="A1:F168"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -26204,9 +26204,69 @@
         <v>8805</v>
       </c>
     </row>
+    <row r="166">
+      <c r="A166" t="str">
+        <v>1.1</v>
+      </c>
+      <c r="B166" t="str">
+        <v>18-07-2025 1:28:44 PM</v>
+      </c>
+      <c r="C166" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D166" t="str">
+        <v>BCL9257C</v>
+      </c>
+      <c r="E166" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F166">
+        <v>10902</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="str">
+        <v>1.2</v>
+      </c>
+      <c r="B167" t="str">
+        <v>18-07-2025 1:28:44 PM</v>
+      </c>
+      <c r="C167" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D167" t="str">
+        <v>BCM0985B</v>
+      </c>
+      <c r="E167" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F167">
+        <v>10048</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="str">
+        <v>1.3</v>
+      </c>
+      <c r="B168" t="str">
+        <v>18-07-2025 1:28:44 PM</v>
+      </c>
+      <c r="C168" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D168" t="str">
+        <v>C077547A</v>
+      </c>
+      <c r="E168" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F168">
+        <v>8244</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F165"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F168"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T08:04:05.325Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F168"/>
+  <dimension ref="A1:F171"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -26264,9 +26264,69 @@
         <v>8244</v>
       </c>
     </row>
+    <row r="169">
+      <c r="A169" t="str">
+        <v>1.1</v>
+      </c>
+      <c r="B169" t="str">
+        <v>18-07-2025 1:34:04 PM</v>
+      </c>
+      <c r="C169" t="str">
+        <v>TN28AK6521</v>
+      </c>
+      <c r="D169" t="str">
+        <v>C061320A</v>
+      </c>
+      <c r="E169" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F169">
+        <v>8599</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="str">
+        <v>1.2</v>
+      </c>
+      <c r="B170" t="str">
+        <v>18-07-2025 1:34:04 PM</v>
+      </c>
+      <c r="C170" t="str">
+        <v>TN28AK6521</v>
+      </c>
+      <c r="D170" t="str">
+        <v>C065864B</v>
+      </c>
+      <c r="E170" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F170">
+        <v>8424</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="str">
+        <v>1.3</v>
+      </c>
+      <c r="B171" t="str">
+        <v>18-07-2025 1:34:04 PM</v>
+      </c>
+      <c r="C171" t="str">
+        <v>TN28AK6521</v>
+      </c>
+      <c r="D171" t="str">
+        <v>C101529B</v>
+      </c>
+      <c r="E171" t="str">
+        <v>SAI</v>
+      </c>
+      <c r="F171">
+        <v>11739</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F168"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F171"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T08:20:30.166Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F171"/>
+  <dimension ref="A1:F174"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -26324,9 +26324,69 @@
         <v>11739</v>
       </c>
     </row>
+    <row r="172">
+      <c r="A172" t="str">
+        <v>1.1</v>
+      </c>
+      <c r="B172" t="str">
+        <v>18-07-2025 1:50:29 PM</v>
+      </c>
+      <c r="C172" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D172" t="str">
+        <v>BCM8546C</v>
+      </c>
+      <c r="E172" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F172">
+        <v>8235</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="str">
+        <v>1.2</v>
+      </c>
+      <c r="B173" t="str">
+        <v>18-07-2025 1:50:29 PM</v>
+      </c>
+      <c r="C173" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D173" t="str">
+        <v>C099800A</v>
+      </c>
+      <c r="E173" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F173">
+        <v>10314</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="str">
+        <v>1.3</v>
+      </c>
+      <c r="B174" t="str">
+        <v>18-07-2025 1:50:29 PM</v>
+      </c>
+      <c r="C174" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D174" t="str">
+        <v>BCN7242B</v>
+      </c>
+      <c r="E174" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F174">
+        <v>10181</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F171"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F174"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 4 new entries added on 2025-07-18T09:01:27.629Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F174"/>
+  <dimension ref="A1:F178"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -26384,9 +26384,89 @@
         <v>10181</v>
       </c>
     </row>
+    <row r="175">
+      <c r="A175" t="str">
+        <v>1.1</v>
+      </c>
+      <c r="B175" t="str">
+        <v>18-07-2025 2:31:26 PM</v>
+      </c>
+      <c r="C175" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D175" t="str">
+        <v>BCM2408A</v>
+      </c>
+      <c r="E175" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F175">
+        <v>10702</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="str">
+        <v>1.2</v>
+      </c>
+      <c r="B176" t="str">
+        <v>18-07-2025 2:31:26 PM</v>
+      </c>
+      <c r="C176" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D176" t="str">
+        <v>C096391B</v>
+      </c>
+      <c r="E176" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F176">
+        <v>10351</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="str">
+        <v>1.3</v>
+      </c>
+      <c r="B177" t="str">
+        <v>18-07-2025 2:31:26 PM</v>
+      </c>
+      <c r="C177" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D177" t="str">
+        <v>BCL9258B</v>
+      </c>
+      <c r="E177" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F177">
+        <v>10492</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="str">
+        <v>1.4</v>
+      </c>
+      <c r="B178" t="str">
+        <v>18-07-2025 2:31:26 PM</v>
+      </c>
+      <c r="C178" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D178" t="str">
+        <v>KGN034A</v>
+      </c>
+      <c r="E178" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F178">
+        <v>9200</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F174"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F178"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T09:23:33.467Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F178"/>
+  <dimension ref="A1:F181"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -26464,9 +26464,69 @@
         <v>9200</v>
       </c>
     </row>
+    <row r="179">
+      <c r="A179" t="str">
+        <v>1.1</v>
+      </c>
+      <c r="B179" t="str">
+        <v>18-07-2025 2:53:33 PM</v>
+      </c>
+      <c r="C179" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D179" t="str">
+        <v>BCN8008A</v>
+      </c>
+      <c r="E179" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F179">
+        <v>8241</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="str">
+        <v>1.2</v>
+      </c>
+      <c r="B180" t="str">
+        <v>18-07-2025 2:53:33 PM</v>
+      </c>
+      <c r="C180" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D180" t="str">
+        <v>C074003C</v>
+      </c>
+      <c r="E180" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F180">
+        <v>8644</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="str">
+        <v>1.3</v>
+      </c>
+      <c r="B181" t="str">
+        <v>18-07-2025 2:53:33 PM</v>
+      </c>
+      <c r="C181" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D181" t="str">
+        <v>AS48095A</v>
+      </c>
+      <c r="E181" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F181">
+        <v>11943</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F178"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F181"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 4 new entries added on 2025-07-18T10:57:06.693Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23604,9 +23604,89 @@
         <v>9294</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>8.1</v>
+      </c>
+      <c r="B36" t="str">
+        <v>18-07-2025 4:27:06 PM</v>
+      </c>
+      <c r="C36" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D36" t="str">
+        <v>C068463C</v>
+      </c>
+      <c r="E36" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F36">
+        <v>8714</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>8.2</v>
+      </c>
+      <c r="B37" t="str">
+        <v>18-07-2025 4:27:06 PM</v>
+      </c>
+      <c r="C37" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D37" t="str">
+        <v>C099026A</v>
+      </c>
+      <c r="E37" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F37">
+        <v>10205</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>8.3</v>
+      </c>
+      <c r="B38" t="str">
+        <v>18-07-2025 4:27:06 PM</v>
+      </c>
+      <c r="C38" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D38" t="str">
+        <v>C087506B</v>
+      </c>
+      <c r="E38" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F38">
+        <v>11159</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>8.4</v>
+      </c>
+      <c r="B39" t="str">
+        <v>18-07-2025 4:27:06 PM</v>
+      </c>
+      <c r="C39" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D39" t="str">
+        <v>BCM2408A</v>
+      </c>
+      <c r="E39" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F39">
+        <v>10702</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F35"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F39"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:00:26.830Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23609,19 +23609,19 @@
         <v>8.1</v>
       </c>
       <c r="B36" t="str">
-        <v>18-07-2025 4:27:06 PM</v>
+        <v>18-07-2025 4:30:26 PM</v>
       </c>
       <c r="C36" t="str">
         <v>TN04AR8167</v>
       </c>
       <c r="D36" t="str">
-        <v>C068463C</v>
+        <v>C057819B</v>
       </c>
       <c r="E36" t="str">
         <v>GWS</v>
       </c>
       <c r="F36">
-        <v>8714</v>
+        <v>8164</v>
       </c>
     </row>
     <row r="37">
@@ -23629,19 +23629,19 @@
         <v>8.2</v>
       </c>
       <c r="B37" t="str">
-        <v>18-07-2025 4:27:06 PM</v>
+        <v>18-07-2025 4:30:26 PM</v>
       </c>
       <c r="C37" t="str">
         <v>TN04AR8167</v>
       </c>
       <c r="D37" t="str">
-        <v>C099026A</v>
+        <v>BCN7247C</v>
       </c>
       <c r="E37" t="str">
         <v>GWS</v>
       </c>
       <c r="F37">
-        <v>10205</v>
+        <v>5270</v>
       </c>
     </row>
     <row r="38">
@@ -23649,44 +23649,24 @@
         <v>8.3</v>
       </c>
       <c r="B38" t="str">
-        <v>18-07-2025 4:27:06 PM</v>
+        <v>18-07-2025 4:30:26 PM</v>
       </c>
       <c r="C38" t="str">
         <v>TN04AR8167</v>
       </c>
       <c r="D38" t="str">
-        <v>C087506B</v>
+        <v>C096391A</v>
       </c>
       <c r="E38" t="str">
         <v>GWS</v>
       </c>
       <c r="F38">
-        <v>11159</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="str">
-        <v>8.4</v>
-      </c>
-      <c r="B39" t="str">
-        <v>18-07-2025 4:27:06 PM</v>
-      </c>
-      <c r="C39" t="str">
-        <v>TN04AR8167</v>
-      </c>
-      <c r="D39" t="str">
-        <v>BCM2408A</v>
-      </c>
-      <c r="E39" t="str">
-        <v>GWS</v>
-      </c>
-      <c r="F39">
-        <v>10702</v>
+        <v>10951</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F39"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F38"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:01:02.117Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -23609,19 +23609,19 @@
         <v>8.1</v>
       </c>
       <c r="B36" t="str">
-        <v>18-07-2025 4:30:26 PM</v>
+        <v>18-07-2025 4:31:01 PM</v>
       </c>
       <c r="C36" t="str">
         <v>TN04AR8167</v>
       </c>
       <c r="D36" t="str">
-        <v>C057819B</v>
+        <v>C070991A</v>
       </c>
       <c r="E36" t="str">
         <v>GWS</v>
       </c>
       <c r="F36">
-        <v>8164</v>
+        <v>9078</v>
       </c>
     </row>
     <row r="37">
@@ -23629,19 +23629,19 @@
         <v>8.2</v>
       </c>
       <c r="B37" t="str">
-        <v>18-07-2025 4:30:26 PM</v>
+        <v>18-07-2025 4:31:01 PM</v>
       </c>
       <c r="C37" t="str">
         <v>TN04AR8167</v>
       </c>
       <c r="D37" t="str">
-        <v>BCN7247C</v>
+        <v>C057819B</v>
       </c>
       <c r="E37" t="str">
         <v>GWS</v>
       </c>
       <c r="F37">
-        <v>5270</v>
+        <v>8164</v>
       </c>
     </row>
     <row r="38">
@@ -23649,19 +23649,19 @@
         <v>8.3</v>
       </c>
       <c r="B38" t="str">
-        <v>18-07-2025 4:30:26 PM</v>
+        <v>18-07-2025 4:31:01 PM</v>
       </c>
       <c r="C38" t="str">
         <v>TN04AR8167</v>
       </c>
       <c r="D38" t="str">
-        <v>C096391A</v>
+        <v>C068951A</v>
       </c>
       <c r="E38" t="str">
         <v>GWS</v>
       </c>
       <c r="F38">
-        <v>10951</v>
+        <v>10424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:04:38.105Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23664,9 +23664,69 @@
         <v>10424</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>8.1</v>
+      </c>
+      <c r="B39" t="str">
+        <v>18-07-2025 4:34:37 PM</v>
+      </c>
+      <c r="C39" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D39" t="str">
+        <v>C068951A</v>
+      </c>
+      <c r="E39" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F39">
+        <v>10424</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>8.2</v>
+      </c>
+      <c r="B40" t="str">
+        <v>18-07-2025 4:34:37 PM</v>
+      </c>
+      <c r="C40" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D40" t="str">
+        <v>C063616A</v>
+      </c>
+      <c r="E40" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F40">
+        <v>10881</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>8.3</v>
+      </c>
+      <c r="B41" t="str">
+        <v>18-07-2025 4:34:37 PM</v>
+      </c>
+      <c r="C41" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D41" t="str">
+        <v>C074003A</v>
+      </c>
+      <c r="E41" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F41">
+        <v>8554</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F38"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F41"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:11:28.165Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23724,9 +23724,69 @@
         <v>8554</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>8.1</v>
+      </c>
+      <c r="B42" t="str">
+        <v>18-07-2025 4:41:27 PM</v>
+      </c>
+      <c r="C42" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D42" t="str">
+        <v>BCL3931B</v>
+      </c>
+      <c r="E42" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F42">
+        <v>8837</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>8.2</v>
+      </c>
+      <c r="B43" t="str">
+        <v>18-07-2025 4:41:27 PM</v>
+      </c>
+      <c r="C43" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D43" t="str">
+        <v>BCN7247C</v>
+      </c>
+      <c r="E43" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F43">
+        <v>5270</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>8.3</v>
+      </c>
+      <c r="B44" t="str">
+        <v>18-07-2025 4:41:27 PM</v>
+      </c>
+      <c r="C44" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D44" t="str">
+        <v>C073932A</v>
+      </c>
+      <c r="E44" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F44">
+        <v>8034</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F41"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F44"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:12:11.565Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -23729,19 +23729,19 @@
         <v>8.1</v>
       </c>
       <c r="B42" t="str">
-        <v>18-07-2025 4:41:27 PM</v>
+        <v>18-07-2025 4:42:10 PM</v>
       </c>
       <c r="C42" t="str">
         <v>TN04AR8167</v>
       </c>
       <c r="D42" t="str">
-        <v>BCL3931B</v>
+        <v>BCM3462C</v>
       </c>
       <c r="E42" t="str">
         <v>GWS</v>
       </c>
       <c r="F42">
-        <v>8837</v>
+        <v>8835</v>
       </c>
     </row>
     <row r="43">
@@ -23749,19 +23749,19 @@
         <v>8.2</v>
       </c>
       <c r="B43" t="str">
-        <v>18-07-2025 4:41:27 PM</v>
+        <v>18-07-2025 4:42:10 PM</v>
       </c>
       <c r="C43" t="str">
         <v>TN04AR8167</v>
       </c>
       <c r="D43" t="str">
-        <v>BCN7247C</v>
+        <v>C099800A</v>
       </c>
       <c r="E43" t="str">
         <v>GWS</v>
       </c>
       <c r="F43">
-        <v>5270</v>
+        <v>10314</v>
       </c>
     </row>
     <row r="44">
@@ -23769,19 +23769,19 @@
         <v>8.3</v>
       </c>
       <c r="B44" t="str">
-        <v>18-07-2025 4:41:27 PM</v>
+        <v>18-07-2025 4:42:10 PM</v>
       </c>
       <c r="C44" t="str">
         <v>TN04AR8167</v>
       </c>
       <c r="D44" t="str">
-        <v>C073932A</v>
+        <v>AS35147C</v>
       </c>
       <c r="E44" t="str">
         <v>GWS</v>
       </c>
       <c r="F44">
-        <v>8034</v>
+        <v>10821</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:15:06.942Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -23726,62 +23726,62 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
       <c r="B42" t="str">
-        <v>18-07-2025 4:42:10 PM</v>
+        <v>18-07-2025 4:45:06 PM</v>
       </c>
       <c r="C42" t="str">
-        <v>TN04AR8167</v>
+        <v>TN04AR8166</v>
       </c>
       <c r="D42" t="str">
-        <v>BCM3462C</v>
+        <v>BCL9258B</v>
       </c>
       <c r="E42" t="str">
         <v>GWS</v>
       </c>
       <c r="F42">
-        <v>8835</v>
+        <v>10492</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>8.2</v>
+        <v>9.2</v>
       </c>
       <c r="B43" t="str">
-        <v>18-07-2025 4:42:10 PM</v>
+        <v>18-07-2025 4:45:06 PM</v>
       </c>
       <c r="C43" t="str">
-        <v>TN04AR8167</v>
+        <v>TN04AR8166</v>
       </c>
       <c r="D43" t="str">
-        <v>C099800A</v>
+        <v>BCM8546C</v>
       </c>
       <c r="E43" t="str">
         <v>GWS</v>
       </c>
       <c r="F43">
-        <v>10314</v>
+        <v>8235</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>8.3</v>
+        <v>9.3</v>
       </c>
       <c r="B44" t="str">
-        <v>18-07-2025 4:42:10 PM</v>
+        <v>18-07-2025 4:45:06 PM</v>
       </c>
       <c r="C44" t="str">
-        <v>TN04AR8167</v>
+        <v>TN04AR8166</v>
       </c>
       <c r="D44" t="str">
-        <v>AS35147C</v>
+        <v>C099736A</v>
       </c>
       <c r="E44" t="str">
         <v>GWS</v>
       </c>
       <c r="F44">
-        <v>10821</v>
+        <v>11843</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:15:38.569Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -23726,62 +23726,62 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>9.1</v>
+        <v>8.1</v>
       </c>
       <c r="B42" t="str">
-        <v>18-07-2025 4:45:06 PM</v>
+        <v>18-07-2025 4:45:38 PM</v>
       </c>
       <c r="C42" t="str">
-        <v>TN04AR8166</v>
+        <v>TN04AR8167</v>
       </c>
       <c r="D42" t="str">
-        <v>BCL9258B</v>
+        <v>BCM6773C</v>
       </c>
       <c r="E42" t="str">
         <v>GWS</v>
       </c>
       <c r="F42">
-        <v>10492</v>
+        <v>7321</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>9.2</v>
+        <v>8.2</v>
       </c>
       <c r="B43" t="str">
-        <v>18-07-2025 4:45:06 PM</v>
+        <v>18-07-2025 4:45:38 PM</v>
       </c>
       <c r="C43" t="str">
-        <v>TN04AR8166</v>
+        <v>TN04AR8167</v>
       </c>
       <c r="D43" t="str">
-        <v>BCM8546C</v>
+        <v>C065863C</v>
       </c>
       <c r="E43" t="str">
         <v>GWS</v>
       </c>
       <c r="F43">
-        <v>8235</v>
+        <v>8644</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>9.3</v>
+        <v>8.3</v>
       </c>
       <c r="B44" t="str">
-        <v>18-07-2025 4:45:06 PM</v>
+        <v>18-07-2025 4:45:38 PM</v>
       </c>
       <c r="C44" t="str">
-        <v>TN04AR8166</v>
+        <v>TN04AR8167</v>
       </c>
       <c r="D44" t="str">
-        <v>C099736A</v>
+        <v>C077439A</v>
       </c>
       <c r="E44" t="str">
         <v>GWS</v>
       </c>
       <c r="F44">
-        <v>11843</v>
+        <v>10895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:20:58.182Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23784,9 +23784,69 @@
         <v>10895</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>8.1</v>
+      </c>
+      <c r="B45" t="str">
+        <v>18-07-2025 4:50:57 PM</v>
+      </c>
+      <c r="C45" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D45" t="str">
+        <v>BCM6888B</v>
+      </c>
+      <c r="E45" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F45">
+        <v>8745</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>8.2</v>
+      </c>
+      <c r="B46" t="str">
+        <v>18-07-2025 4:50:57 PM</v>
+      </c>
+      <c r="C46" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D46" t="str">
+        <v>C096391A</v>
+      </c>
+      <c r="E46" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F46">
+        <v>10951</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>8.3</v>
+      </c>
+      <c r="B47" t="str">
+        <v>18-07-2025 4:50:57 PM</v>
+      </c>
+      <c r="C47" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D47" t="str">
+        <v>C101291B</v>
+      </c>
+      <c r="E47" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F47">
+        <v>9281</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F44"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F47"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:21:37.142Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -23786,62 +23786,62 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
       <c r="B45" t="str">
-        <v>18-07-2025 4:50:57 PM</v>
+        <v>18-07-2025 4:51:36 PM</v>
       </c>
       <c r="C45" t="str">
-        <v>TN04AR8167</v>
+        <v>TN04AR8166</v>
       </c>
       <c r="D45" t="str">
-        <v>BCM6888B</v>
+        <v>C053304B</v>
       </c>
       <c r="E45" t="str">
         <v>GWS</v>
       </c>
       <c r="F45">
-        <v>8745</v>
+        <v>10104</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>8.2</v>
+        <v>9.2</v>
       </c>
       <c r="B46" t="str">
-        <v>18-07-2025 4:50:57 PM</v>
+        <v>18-07-2025 4:51:36 PM</v>
       </c>
       <c r="C46" t="str">
-        <v>TN04AR8167</v>
+        <v>TN04AR8166</v>
       </c>
       <c r="D46" t="str">
-        <v>C096391A</v>
+        <v>C078812B</v>
       </c>
       <c r="E46" t="str">
         <v>GWS</v>
       </c>
       <c r="F46">
-        <v>10951</v>
+        <v>11004</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>8.3</v>
+        <v>9.3</v>
       </c>
       <c r="B47" t="str">
-        <v>18-07-2025 4:50:57 PM</v>
+        <v>18-07-2025 4:51:36 PM</v>
       </c>
       <c r="C47" t="str">
-        <v>TN04AR8167</v>
+        <v>TN04AR8166</v>
       </c>
       <c r="D47" t="str">
-        <v>C101291B</v>
+        <v>C075553A</v>
       </c>
       <c r="E47" t="str">
         <v>GWS</v>
       </c>
       <c r="F47">
-        <v>9281</v>
+        <v>10758</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:22:17.427Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -23786,62 +23786,62 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>9.1</v>
+        <v>10.1</v>
       </c>
       <c r="B45" t="str">
-        <v>18-07-2025 4:51:36 PM</v>
+        <v>18-07-2025 4:52:17 PM</v>
       </c>
       <c r="C45" t="str">
-        <v>TN04AR8166</v>
+        <v>TN04AJ6984</v>
       </c>
       <c r="D45" t="str">
-        <v>C053304B</v>
+        <v>C065863B</v>
       </c>
       <c r="E45" t="str">
-        <v>GWS</v>
+        <v>MST</v>
       </c>
       <c r="F45">
-        <v>10104</v>
+        <v>8614</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>9.2</v>
+        <v>10.2</v>
       </c>
       <c r="B46" t="str">
-        <v>18-07-2025 4:51:36 PM</v>
+        <v>18-07-2025 4:52:17 PM</v>
       </c>
       <c r="C46" t="str">
-        <v>TN04AR8166</v>
+        <v>TN04AJ6984</v>
       </c>
       <c r="D46" t="str">
-        <v>C078812B</v>
+        <v>C063616A</v>
       </c>
       <c r="E46" t="str">
-        <v>GWS</v>
+        <v>MST</v>
       </c>
       <c r="F46">
-        <v>11004</v>
+        <v>10881</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>9.3</v>
+        <v>10.3</v>
       </c>
       <c r="B47" t="str">
-        <v>18-07-2025 4:51:36 PM</v>
+        <v>18-07-2025 4:52:17 PM</v>
       </c>
       <c r="C47" t="str">
-        <v>TN04AR8166</v>
+        <v>TN04AJ6984</v>
       </c>
       <c r="D47" t="str">
-        <v>C075553A</v>
+        <v>BCN7247C</v>
       </c>
       <c r="E47" t="str">
-        <v>GWS</v>
+        <v>MST</v>
       </c>
       <c r="F47">
-        <v>10758</v>
+        <v>5270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:24:39.068Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -23786,62 +23786,62 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>10.1</v>
+        <v>8.1</v>
       </c>
       <c r="B45" t="str">
-        <v>18-07-2025 4:52:17 PM</v>
+        <v>18-07-2025 4:54:38 PM</v>
       </c>
       <c r="C45" t="str">
-        <v>TN04AJ6984</v>
+        <v>TN04AR8167</v>
       </c>
       <c r="D45" t="str">
-        <v>C065863B</v>
+        <v>C077440A</v>
       </c>
       <c r="E45" t="str">
-        <v>MST</v>
+        <v>GWS</v>
       </c>
       <c r="F45">
-        <v>8614</v>
+        <v>10375</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>10.2</v>
+        <v>8.2</v>
       </c>
       <c r="B46" t="str">
-        <v>18-07-2025 4:52:17 PM</v>
+        <v>18-07-2025 4:54:38 PM</v>
       </c>
       <c r="C46" t="str">
-        <v>TN04AJ6984</v>
+        <v>TN04AR8167</v>
       </c>
       <c r="D46" t="str">
-        <v>C063616A</v>
+        <v>BCN6657</v>
       </c>
       <c r="E46" t="str">
-        <v>MST</v>
+        <v>GWS</v>
       </c>
       <c r="F46">
-        <v>10881</v>
+        <v>13365</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>10.3</v>
+        <v>8.3</v>
       </c>
       <c r="B47" t="str">
-        <v>18-07-2025 4:52:17 PM</v>
+        <v>18-07-2025 4:54:38 PM</v>
       </c>
       <c r="C47" t="str">
-        <v>TN04AJ6984</v>
+        <v>TN04AR8167</v>
       </c>
       <c r="D47" t="str">
-        <v>BCN7247C</v>
+        <v>C057819B</v>
       </c>
       <c r="E47" t="str">
-        <v>MST</v>
+        <v>GWS</v>
       </c>
       <c r="F47">
-        <v>5270</v>
+        <v>8164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:25:09.535Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -23786,62 +23786,62 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>8.1</v>
+        <v>11.1</v>
       </c>
       <c r="B45" t="str">
-        <v>18-07-2025 4:54:38 PM</v>
+        <v>18-07-2025 4:55:09 PM</v>
       </c>
       <c r="C45" t="str">
-        <v>TN04AR8167</v>
+        <v>TN28AK9553</v>
       </c>
       <c r="D45" t="str">
-        <v>C077440A</v>
+        <v>BCG7096A</v>
       </c>
       <c r="E45" t="str">
-        <v>GWS</v>
+        <v>SCT</v>
       </c>
       <c r="F45">
-        <v>10375</v>
+        <v>8839</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>8.2</v>
+        <v>11.2</v>
       </c>
       <c r="B46" t="str">
-        <v>18-07-2025 4:54:38 PM</v>
+        <v>18-07-2025 4:55:09 PM</v>
       </c>
       <c r="C46" t="str">
-        <v>TN04AR8167</v>
+        <v>TN28AK9553</v>
       </c>
       <c r="D46" t="str">
-        <v>BCN6657</v>
+        <v>C099954C</v>
       </c>
       <c r="E46" t="str">
-        <v>GWS</v>
+        <v>SCT</v>
       </c>
       <c r="F46">
-        <v>13365</v>
+        <v>8484</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>8.3</v>
+        <v>11.3</v>
       </c>
       <c r="B47" t="str">
-        <v>18-07-2025 4:54:38 PM</v>
+        <v>18-07-2025 4:55:09 PM</v>
       </c>
       <c r="C47" t="str">
-        <v>TN04AR8167</v>
+        <v>TN28AK9553</v>
       </c>
       <c r="D47" t="str">
-        <v>C057819B</v>
+        <v>C099954AA</v>
       </c>
       <c r="E47" t="str">
-        <v>GWS</v>
+        <v>SCT</v>
       </c>
       <c r="F47">
-        <v>8164</v>
+        <v>6350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:25:42.734Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23844,9 +23844,69 @@
         <v>6350</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>11.1</v>
+      </c>
+      <c r="B48" t="str">
+        <v>18-07-2025 4:55:41 PM</v>
+      </c>
+      <c r="C48" t="str">
+        <v>TN28AK9553</v>
+      </c>
+      <c r="D48" t="str">
+        <v>C075553B</v>
+      </c>
+      <c r="E48" t="str">
+        <v>SCT</v>
+      </c>
+      <c r="F48">
+        <v>10658</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>11.2</v>
+      </c>
+      <c r="B49" t="str">
+        <v>18-07-2025 4:55:41 PM</v>
+      </c>
+      <c r="C49" t="str">
+        <v>TN28AK9553</v>
+      </c>
+      <c r="D49" t="str">
+        <v>C092733B</v>
+      </c>
+      <c r="E49" t="str">
+        <v>SCT</v>
+      </c>
+      <c r="F49">
+        <v>10815</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>11.3</v>
+      </c>
+      <c r="B50" t="str">
+        <v>18-07-2025 4:55:41 PM</v>
+      </c>
+      <c r="C50" t="str">
+        <v>TN28AK9553</v>
+      </c>
+      <c r="D50" t="str">
+        <v>KGM113B</v>
+      </c>
+      <c r="E50" t="str">
+        <v>SCT</v>
+      </c>
+      <c r="F50">
+        <v>10243</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F47"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F50"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:34:03.324Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23904,9 +23904,69 @@
         <v>10243</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>8.1</v>
+      </c>
+      <c r="B51" t="str">
+        <v>18-07-2025 5:04:02 PM</v>
+      </c>
+      <c r="C51" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D51" t="str">
+        <v>BCN9423B</v>
+      </c>
+      <c r="E51" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F51">
+        <v>10514</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>8.2</v>
+      </c>
+      <c r="B52" t="str">
+        <v>18-07-2025 5:04:02 PM</v>
+      </c>
+      <c r="C52" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D52" t="str">
+        <v>C068463C</v>
+      </c>
+      <c r="E52" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F52">
+        <v>8714</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>8.3</v>
+      </c>
+      <c r="B53" t="str">
+        <v>18-07-2025 5:04:02 PM</v>
+      </c>
+      <c r="C53" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D53" t="str">
+        <v>C080045B</v>
+      </c>
+      <c r="E53" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F53">
+        <v>8397</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F50"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F53"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:34:38.314Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -23906,62 +23906,62 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
       <c r="B51" t="str">
-        <v>18-07-2025 5:04:02 PM</v>
+        <v>18-07-2025 5:04:37 PM</v>
       </c>
       <c r="C51" t="str">
-        <v>TN04AR8167</v>
+        <v>TN88H1179</v>
       </c>
       <c r="D51" t="str">
-        <v>BCN9423B</v>
+        <v>C099881B</v>
       </c>
       <c r="E51" t="str">
-        <v>GWS</v>
+        <v>SAI</v>
       </c>
       <c r="F51">
-        <v>10514</v>
+        <v>11439</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>8.2</v>
+        <v>9.2</v>
       </c>
       <c r="B52" t="str">
-        <v>18-07-2025 5:04:02 PM</v>
+        <v>18-07-2025 5:04:37 PM</v>
       </c>
       <c r="C52" t="str">
-        <v>TN04AR8167</v>
+        <v>TN88H1179</v>
       </c>
       <c r="D52" t="str">
-        <v>C068463C</v>
+        <v>C099954AA</v>
       </c>
       <c r="E52" t="str">
-        <v>GWS</v>
+        <v>SAI</v>
       </c>
       <c r="F52">
-        <v>8714</v>
+        <v>6350</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>8.3</v>
+        <v>9.3</v>
       </c>
       <c r="B53" t="str">
-        <v>18-07-2025 5:04:02 PM</v>
+        <v>18-07-2025 5:04:37 PM</v>
       </c>
       <c r="C53" t="str">
-        <v>TN04AR8167</v>
+        <v>TN88H1179</v>
       </c>
       <c r="D53" t="str">
-        <v>C080045B</v>
+        <v>BCL1144</v>
       </c>
       <c r="E53" t="str">
-        <v>GWS</v>
+        <v>SAI</v>
       </c>
       <c r="F53">
-        <v>8397</v>
+        <v>13638</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T11:35:19.726Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -23906,62 +23906,62 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>9.1</v>
+        <v>8.1</v>
       </c>
       <c r="B51" t="str">
-        <v>18-07-2025 5:04:37 PM</v>
+        <v>18-07-2025 5:05:19 PM</v>
       </c>
       <c r="C51" t="str">
-        <v>TN88H1179</v>
+        <v>TN04AR8167</v>
       </c>
       <c r="D51" t="str">
-        <v>C099881B</v>
+        <v>C062523B</v>
       </c>
       <c r="E51" t="str">
-        <v>SAI</v>
+        <v>GWS</v>
       </c>
       <c r="F51">
-        <v>11439</v>
+        <v>10174</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>9.2</v>
+        <v>8.2</v>
       </c>
       <c r="B52" t="str">
-        <v>18-07-2025 5:04:37 PM</v>
+        <v>18-07-2025 5:05:19 PM</v>
       </c>
       <c r="C52" t="str">
-        <v>TN88H1179</v>
+        <v>TN04AR8167</v>
       </c>
       <c r="D52" t="str">
-        <v>C099954AA</v>
+        <v>C063953A</v>
       </c>
       <c r="E52" t="str">
-        <v>SAI</v>
+        <v>GWS</v>
       </c>
       <c r="F52">
-        <v>6350</v>
+        <v>10825</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>9.3</v>
+        <v>8.3</v>
       </c>
       <c r="B53" t="str">
-        <v>18-07-2025 5:04:37 PM</v>
+        <v>18-07-2025 5:05:19 PM</v>
       </c>
       <c r="C53" t="str">
-        <v>TN88H1179</v>
+        <v>TN04AR8167</v>
       </c>
       <c r="D53" t="str">
-        <v>BCL1144</v>
+        <v>C093361A</v>
       </c>
       <c r="E53" t="str">
-        <v>SAI</v>
+        <v>GWS</v>
       </c>
       <c r="F53">
-        <v>13638</v>
+        <v>9824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T12:01:57.489Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23964,9 +23964,69 @@
         <v>9824</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>8.1</v>
+      </c>
+      <c r="B54" t="str">
+        <v>18-07-2025 5:31:56 PM</v>
+      </c>
+      <c r="C54" t="str">
+        <v>TN03U0432</v>
+      </c>
+      <c r="D54" t="str">
+        <v>BCL9256A</v>
+      </c>
+      <c r="E54" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F54">
+        <v>10162</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>8.2</v>
+      </c>
+      <c r="B55" t="str">
+        <v>18-07-2025 5:31:56 PM</v>
+      </c>
+      <c r="C55" t="str">
+        <v>TN03U0432</v>
+      </c>
+      <c r="D55" t="str">
+        <v>BCM4941A</v>
+      </c>
+      <c r="E55" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F55">
+        <v>10135</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>8.3</v>
+      </c>
+      <c r="B56" t="str">
+        <v>18-07-2025 5:31:56 PM</v>
+      </c>
+      <c r="C56" t="str">
+        <v>TN03U0432</v>
+      </c>
+      <c r="D56" t="str">
+        <v>BCN2078A</v>
+      </c>
+      <c r="E56" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F56">
+        <v>7635</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F53"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F56"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T12:02:31.432Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -23966,62 +23966,62 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
       <c r="B54" t="str">
-        <v>18-07-2025 5:31:56 PM</v>
+        <v>18-07-2025 5:32:30 PM</v>
       </c>
       <c r="C54" t="str">
-        <v>TN03U0432</v>
+        <v>TN04AR8167</v>
       </c>
       <c r="D54" t="str">
-        <v>BCL9256A</v>
+        <v>BCG7096B</v>
       </c>
       <c r="E54" t="str">
-        <v>MPT</v>
+        <v>GWS</v>
       </c>
       <c r="F54">
-        <v>10162</v>
+        <v>8659</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>8.2</v>
+        <v>9.2</v>
       </c>
       <c r="B55" t="str">
-        <v>18-07-2025 5:31:56 PM</v>
+        <v>18-07-2025 5:32:30 PM</v>
       </c>
       <c r="C55" t="str">
-        <v>TN03U0432</v>
+        <v>TN04AR8167</v>
       </c>
       <c r="D55" t="str">
-        <v>BCM4941A</v>
+        <v>C101233A</v>
       </c>
       <c r="E55" t="str">
-        <v>MPT</v>
+        <v>GWS</v>
       </c>
       <c r="F55">
-        <v>10135</v>
+        <v>11149</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>8.3</v>
+        <v>9.3</v>
       </c>
       <c r="B56" t="str">
-        <v>18-07-2025 5:31:56 PM</v>
+        <v>18-07-2025 5:32:30 PM</v>
       </c>
       <c r="C56" t="str">
-        <v>TN03U0432</v>
+        <v>TN04AR8167</v>
       </c>
       <c r="D56" t="str">
-        <v>BCN2078A</v>
+        <v>C101234B</v>
       </c>
       <c r="E56" t="str">
-        <v>MPT</v>
+        <v>GWS</v>
       </c>
       <c r="F56">
-        <v>7635</v>
+        <v>8191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T12:03:06.351Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -23966,62 +23966,62 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>9.1</v>
+        <v>10.1</v>
       </c>
       <c r="B54" t="str">
-        <v>18-07-2025 5:32:30 PM</v>
+        <v>18-07-2025 5:33:04 PM</v>
       </c>
       <c r="C54" t="str">
-        <v>TN04AR8167</v>
+        <v>TN88L9619</v>
       </c>
       <c r="D54" t="str">
-        <v>BCG7096B</v>
+        <v>BCM7923B</v>
       </c>
       <c r="E54" t="str">
-        <v>GWS</v>
+        <v>MSMD</v>
       </c>
       <c r="F54">
-        <v>8659</v>
+        <v>8915</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>9.2</v>
+        <v>10.2</v>
       </c>
       <c r="B55" t="str">
-        <v>18-07-2025 5:32:30 PM</v>
+        <v>18-07-2025 5:33:04 PM</v>
       </c>
       <c r="C55" t="str">
-        <v>TN04AR8167</v>
+        <v>TN88L9619</v>
       </c>
       <c r="D55" t="str">
-        <v>C101233A</v>
+        <v>C062523B</v>
       </c>
       <c r="E55" t="str">
-        <v>GWS</v>
+        <v>MSMD</v>
       </c>
       <c r="F55">
-        <v>11149</v>
+        <v>10174</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>9.3</v>
+        <v>10.3</v>
       </c>
       <c r="B56" t="str">
-        <v>18-07-2025 5:32:30 PM</v>
+        <v>18-07-2025 5:33:04 PM</v>
       </c>
       <c r="C56" t="str">
-        <v>TN04AR8167</v>
+        <v>TN88L9619</v>
       </c>
       <c r="D56" t="str">
-        <v>C101234B</v>
+        <v>C078750B</v>
       </c>
       <c r="E56" t="str">
-        <v>GWS</v>
+        <v>MSMD</v>
       </c>
       <c r="F56">
-        <v>8191</v>
+        <v>8691</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 4 new entries added on 2025-07-18T13:31:59.845Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24024,9 +24024,89 @@
         <v>8691</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>8.4</v>
+      </c>
+      <c r="B57" t="str">
+        <v>18-07-2025 7:01:58 PM</v>
+      </c>
+      <c r="C57" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D57" t="str">
+        <v>BCM6772B</v>
+      </c>
+      <c r="E57" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F57">
+        <v>9965</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>8.5</v>
+      </c>
+      <c r="B58" t="str">
+        <v>18-07-2025 7:01:58 PM</v>
+      </c>
+      <c r="C58" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D58" t="str">
+        <v>C087504B</v>
+      </c>
+      <c r="E58" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F58">
+        <v>9615</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>8.6</v>
+      </c>
+      <c r="B59" t="str">
+        <v>18-07-2025 7:01:58 PM</v>
+      </c>
+      <c r="C59" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D59" t="str">
+        <v>C068459</v>
+      </c>
+      <c r="E59" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F59">
+        <v>6980</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>8.7</v>
+      </c>
+      <c r="B60" t="str">
+        <v>18-07-2025 7:01:58 PM</v>
+      </c>
+      <c r="C60" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D60" t="str">
+        <v>BCM6773C</v>
+      </c>
+      <c r="E60" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F60">
+        <v>7321</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F56"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F60"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-18T13:48:16.291Z
</commit_message>
<xml_diff>
--- a/M.V. POAVOSA ACE V.2506W.xlsx
+++ b/M.V. POAVOSA ACE V.2506W.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24104,9 +24104,69 @@
         <v>7321</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>8.4</v>
+      </c>
+      <c r="B61" t="str">
+        <v>18-07-2025 7:18:15 PM</v>
+      </c>
+      <c r="C61" t="str">
+        <v>TN04AK0675</v>
+      </c>
+      <c r="D61" t="str">
+        <v>BCM6773C</v>
+      </c>
+      <c r="E61" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F61">
+        <v>7321</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>8.5</v>
+      </c>
+      <c r="B62" t="str">
+        <v>18-07-2025 7:18:15 PM</v>
+      </c>
+      <c r="C62" t="str">
+        <v>TN04AK0675</v>
+      </c>
+      <c r="D62" t="str">
+        <v>C087504B</v>
+      </c>
+      <c r="E62" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F62">
+        <v>9615</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>8.6</v>
+      </c>
+      <c r="B63" t="str">
+        <v>18-07-2025 7:18:15 PM</v>
+      </c>
+      <c r="C63" t="str">
+        <v>TN04AK0675</v>
+      </c>
+      <c r="D63" t="str">
+        <v>BCN9423B</v>
+      </c>
+      <c r="E63" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F63">
+        <v>10514</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F60"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F63"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>